<commit_message>
Setup testkit for {{#each}} support
</commit_message>
<xml_diff>
--- a/test/data/people.xlsx
+++ b/test/data/people.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t xml:space="preserve">Example Person</t>
   </si>
@@ -50,19 +50,19 @@
     <t xml:space="preserve">{{people.0.phone}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{#each people}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{name}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{sex}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{email}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{address.street}}, {{address.city}}, {{address.zipcode}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{phone}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{/each}}</t>
@@ -170,7 +170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -187,7 +187,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,7 +274,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -336,10 +340,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -348,30 +352,37 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AMJ1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Repeaters are now supported
</commit_message>
<xml_diff>
--- a/test/data/people.xlsx
+++ b/test/data/people.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t xml:space="preserve">Example Person</t>
   </si>
@@ -50,22 +50,16 @@
     <t xml:space="preserve">{{people.0.phone}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{#each people}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{name}}</t>
+    <t xml:space="preserve">{{#each people}}{{name}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{email}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{address.street}}, {{address.city}}, {{address.zipcode}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{{phone}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{/each}}</t>
+    <t xml:space="preserve">{{address.street}}, {{address.city}}, {{address.zipcode}}{{/each}}</t>
   </si>
 </sst>
 </file>
@@ -80,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -101,12 +96,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -114,6 +111,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -170,12 +168,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -184,10 +182,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,13 +269,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -340,16 +331,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="1:2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,41 +350,32 @@
         <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AMJ1" s="4"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
REFACTOR: Major refactor to use the better supported xlsx-populate library instead of xlsx (supports styling + media inserts such as pictures) REFACTOR: Switched to using a promise async reader
</commit_message>
<xml_diff>
--- a/test/data/people.xlsx
+++ b/test/data/people.xlsx
@@ -181,11 +181,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,6 +273,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -284,7 +287,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -292,7 +295,7 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -300,7 +303,7 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -308,7 +311,7 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -339,36 +342,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="AMI1" s="3"/>
+      <c r="AMJ1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for ES6 templates Added Debug NPM support
</commit_message>
<xml_diff>
--- a/test/data/people.xlsx
+++ b/test/data/people.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Person" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">Example Person</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">{{people.0.phone}}</t>
   </si>
   <si>
+    <t xml:space="preserve">Dob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{#each people}}{{name}}</t>
   </si>
   <si>
@@ -59,7 +65,13 @@
     <t xml:space="preserve">{{phone}}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{address.street}}, {{address.city}}, {{address.zipcode}}{{/each}}</t>
+    <t xml:space="preserve">{{address.street}}, {{address.city}}, {{address.zipcode}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${dob}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${Math.floor((new Date().getTime() - dob.getTime()) / (1000 * 60 * 60 * 24 * 365.2425))}{{/each}}</t>
   </si>
 </sst>
 </file>
@@ -191,12 +203,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -268,13 +280,13 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,7 +333,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -334,16 +346,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,27 +371,39 @@
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="AMI1" s="3"/>
       <c r="AMJ1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>